<commit_message>
OTreeAlg: frac_t -> struct using gcd -overflows-> double consistentNodes as a sorted list instead of a set of pointers (nondeterminism)
</commit_message>
<xml_diff>
--- a/data/Mealy_R100.xlsx
+++ b/data/Mealy_R100.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="10515" windowHeight="4695" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="10515" windowHeight="4695"/>
   </bookViews>
   <sheets>
-    <sheet name="Mealy_R5" sheetId="1" r:id="rId1"/>
+    <sheet name="Mealy_R100" sheetId="1" r:id="rId1"/>
     <sheet name="TeacherDFSM" sheetId="2" r:id="rId2"/>
     <sheet name="TeacherRL" sheetId="3" r:id="rId3"/>
     <sheet name="TeacherBB" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Moore_R10_PDS" localSheetId="0">Mealy_R5!$A$1:$K$40</definedName>
+    <definedName name="Moore_R10_PDS" localSheetId="0">Mealy_R100!$A$1:$K$40</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -704,7 +704,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Mealy_R5!$B$1</c:f>
+              <c:f>Mealy_R100!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -715,7 +715,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Mealy_R5!$G$2:$H$14</c:f>
+              <c:f>Mealy_R100!$G$2:$H$14</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="13"/>
                 <c:lvl>
@@ -796,7 +796,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Mealy_R5!$B$2:$B$14</c:f>
+              <c:f>Mealy_R100!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -837,7 +837,7 @@
                   <c:v>5712</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3247</c:v>
+                  <c:v>3177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -849,7 +849,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Mealy_R5!$C$1</c:f>
+              <c:f>Mealy_R100!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -860,7 +860,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Mealy_R5!$G$2:$H$14</c:f>
+              <c:f>Mealy_R100!$G$2:$H$14</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="13"/>
                 <c:lvl>
@@ -941,7 +941,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Mealy_R5!$C$2:$C$14</c:f>
+              <c:f>Mealy_R100!$C$2:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -982,7 +982,7 @@
                   <c:v>5712</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6180</c:v>
+                  <c:v>6028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -994,7 +994,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Mealy_R5!$E$1</c:f>
+              <c:f>Mealy_R100!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1005,7 +1005,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Mealy_R5!$G$2:$H$14</c:f>
+              <c:f>Mealy_R100!$G$2:$H$14</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="13"/>
                 <c:lvl>
@@ -1086,7 +1086,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Mealy_R5!$E$2:$E$14</c:f>
+              <c:f>Mealy_R100!$E$2:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1127,7 +1127,7 @@
                   <c:v>39062</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25356</c:v>
+                  <c:v>24669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1144,8 +1144,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="18300928"/>
-        <c:axId val="18302464"/>
+        <c:axId val="131195648"/>
+        <c:axId val="131197184"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1155,7 +1155,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Mealy_R5!$D$1</c:f>
+              <c:f>Mealy_R100!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1166,7 +1166,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Mealy_R5!$D$2:$D$14</c:f>
+              <c:f>Mealy_R100!$D$2:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1224,11 +1224,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="18318464"/>
-        <c:axId val="18304000"/>
+        <c:axId val="131467136"/>
+        <c:axId val="131465216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="18300928"/>
+        <c:axId val="131195648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1237,7 +1237,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="18302464"/>
+        <c:crossAx val="131197184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1245,7 +1245,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18302464"/>
+        <c:axId val="131197184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1256,12 +1256,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="18300928"/>
+        <c:crossAx val="131195648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="18304000"/>
+        <c:axId val="131465216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1283,19 +1283,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="18318464"/>
+        <c:crossAx val="131467136"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="18318464"/>
+        <c:axId val="131467136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1304,7 +1303,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="18304000"/>
+        <c:crossAx val="131465216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1314,7 +1313,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1349,7 +1347,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Mealy_R5!$B$1</c:f>
+              <c:f>Mealy_R100!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1360,7 +1358,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Mealy_R5!$G$15:$H$27</c:f>
+              <c:f>Mealy_R100!$G$15:$H$27</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="13"/>
                 <c:lvl>
@@ -1441,7 +1439,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Mealy_R5!$B$15:$B$27</c:f>
+              <c:f>Mealy_R100!$B$15:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1482,7 +1480,7 @@
                   <c:v>5854</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3247</c:v>
+                  <c:v>3177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1494,7 +1492,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Mealy_R5!$C$1</c:f>
+              <c:f>Mealy_R100!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1505,7 +1503,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Mealy_R5!$G$15:$H$27</c:f>
+              <c:f>Mealy_R100!$G$15:$H$27</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="13"/>
                 <c:lvl>
@@ -1586,7 +1584,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Mealy_R5!$C$15:$C$27</c:f>
+              <c:f>Mealy_R100!$C$15:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1627,7 +1625,7 @@
                   <c:v>5854</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6180</c:v>
+                  <c:v>6028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1639,7 +1637,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Mealy_R5!$E$1</c:f>
+              <c:f>Mealy_R100!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1650,7 +1648,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Mealy_R5!$G$15:$H$27</c:f>
+              <c:f>Mealy_R100!$G$15:$H$27</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="13"/>
                 <c:lvl>
@@ -1731,7 +1729,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Mealy_R5!$E$15:$E$27</c:f>
+              <c:f>Mealy_R100!$E$15:$E$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1772,7 +1770,7 @@
                   <c:v>40378</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25356</c:v>
+                  <c:v>24669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1789,8 +1787,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="18350080"/>
-        <c:axId val="18351616"/>
+        <c:axId val="131810816"/>
+        <c:axId val="131812352"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1800,7 +1798,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Mealy_R5!$D$1</c:f>
+              <c:f>Mealy_R100!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1811,7 +1809,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Mealy_R5!$D$15:$D$27</c:f>
+              <c:f>Mealy_R100!$D$15:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1869,11 +1867,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="18367616"/>
-        <c:axId val="18353152"/>
+        <c:axId val="131832448"/>
+        <c:axId val="131830528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="18350080"/>
+        <c:axId val="131810816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1882,7 +1880,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="18351616"/>
+        <c:crossAx val="131812352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1890,7 +1888,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18351616"/>
+        <c:axId val="131812352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1901,12 +1899,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="18350080"/>
+        <c:crossAx val="131810816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="18353152"/>
+        <c:axId val="131830528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1928,19 +1926,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="18367616"/>
+        <c:crossAx val="131832448"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="18367616"/>
+        <c:axId val="131832448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1949,7 +1946,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="18353152"/>
+        <c:crossAx val="131830528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1959,7 +1956,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1994,7 +1990,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Mealy_R5!$B$1</c:f>
+              <c:f>Mealy_R100!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2005,7 +2001,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Mealy_R5!$G$28:$H$40</c:f>
+              <c:f>Mealy_R100!$G$28:$H$40</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="13"/>
                 <c:lvl>
@@ -2086,7 +2082,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Mealy_R5!$B$28:$B$40</c:f>
+              <c:f>Mealy_R100!$B$28:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2127,7 +2123,7 @@
                   <c:v>5773</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3247</c:v>
+                  <c:v>3177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2139,7 +2135,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Mealy_R5!$C$1</c:f>
+              <c:f>Mealy_R100!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2150,7 +2146,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Mealy_R5!$G$28:$H$40</c:f>
+              <c:f>Mealy_R100!$G$28:$H$40</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="13"/>
                 <c:lvl>
@@ -2231,7 +2227,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Mealy_R5!$C$28:$C$40</c:f>
+              <c:f>Mealy_R100!$C$28:$C$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2272,7 +2268,7 @@
                   <c:v>5773</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6180</c:v>
+                  <c:v>6028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2284,7 +2280,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Mealy_R5!$E$1</c:f>
+              <c:f>Mealy_R100!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2295,7 +2291,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Mealy_R5!$G$28:$H$40</c:f>
+              <c:f>Mealy_R100!$G$28:$H$40</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="13"/>
                 <c:lvl>
@@ -2376,7 +2372,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Mealy_R5!$E$28:$E$40</c:f>
+              <c:f>Mealy_R100!$E$28:$E$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2417,7 +2413,7 @@
                   <c:v>5964</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6180</c:v>
+                  <c:v>6028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2434,8 +2430,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="18440960"/>
-        <c:axId val="18442496"/>
+        <c:axId val="131868928"/>
+        <c:axId val="131883008"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2445,7 +2441,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Mealy_R5!$D$1</c:f>
+              <c:f>Mealy_R100!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2456,7 +2452,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Mealy_R5!$D$28:$D$40</c:f>
+              <c:f>Mealy_R100!$D$28:$D$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2514,11 +2510,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="18450304"/>
-        <c:axId val="18448384"/>
+        <c:axId val="131886464"/>
+        <c:axId val="131884544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="18440960"/>
+        <c:axId val="131868928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2527,7 +2523,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="18442496"/>
+        <c:crossAx val="131883008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2535,7 +2531,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18442496"/>
+        <c:axId val="131883008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2546,12 +2542,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="18440960"/>
+        <c:crossAx val="131868928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="18448384"/>
+        <c:axId val="131884544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2573,19 +2569,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="18450304"/>
+        <c:crossAx val="131886464"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="18450304"/>
+        <c:axId val="131886464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2594,7 +2589,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="18448384"/>
+        <c:crossAx val="131884544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2604,7 +2599,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2640,7 +2634,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="82" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2705,7 +2699,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9302338" cy="6011883"/>
+    <xdr:ext cx="9326563" cy="6032500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graf 1"/>
@@ -3021,8 +3015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3415,16 +3409,16 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>3247</v>
+        <v>3177</v>
       </c>
       <c r="C14">
-        <v>6180</v>
+        <v>6028</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>25356</v>
+        <v>24669</v>
       </c>
       <c r="F14" t="s">
         <v>29</v>
@@ -3783,16 +3777,16 @@
         <v>1</v>
       </c>
       <c r="B27">
-        <v>3247</v>
+        <v>3177</v>
       </c>
       <c r="C27">
-        <v>6180</v>
+        <v>6028</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>25356</v>
+        <v>24669</v>
       </c>
       <c r="F27" t="s">
         <v>29</v>
@@ -4187,16 +4181,16 @@
         <v>1</v>
       </c>
       <c r="B40">
-        <v>3247</v>
+        <v>3177</v>
       </c>
       <c r="C40">
-        <v>6180</v>
+        <v>6028</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40">
-        <v>6180</v>
+        <v>6028</v>
       </c>
       <c r="F40" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
OTreeAlg: confirm (SVS) instead of identify (ADS) for next states of extra states
</commit_message>
<xml_diff>
--- a/data/Mealy_R100.xlsx
+++ b/data/Mealy_R100.xlsx
@@ -837,7 +837,7 @@
                   <c:v>5712</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3177</c:v>
+                  <c:v>2875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -982,7 +982,7 @@
                   <c:v>5712</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6028</c:v>
+                  <c:v>6040</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,7 +1127,7 @@
                   <c:v>39062</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24669</c:v>
+                  <c:v>22008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1283,6 +1283,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1313,6 +1314,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1480,7 +1482,7 @@
                   <c:v>5854</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3177</c:v>
+                  <c:v>2875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1625,7 +1627,7 @@
                   <c:v>5854</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6028</c:v>
+                  <c:v>6040</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1770,7 +1772,7 @@
                   <c:v>40378</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24669</c:v>
+                  <c:v>22008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1926,6 +1928,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1956,6 +1959,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2123,7 +2127,7 @@
                   <c:v>5773</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3177</c:v>
+                  <c:v>2875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2268,7 +2272,7 @@
                   <c:v>5773</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6028</c:v>
+                  <c:v>6040</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2413,7 +2417,7 @@
                   <c:v>5964</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6028</c:v>
+                  <c:v>6040</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2569,6 +2573,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2599,6 +2604,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2699,7 +2705,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9326563" cy="6032500"/>
+    <xdr:ext cx="9304299" cy="6017012"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graf 1"/>
@@ -3015,8 +3021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3409,16 +3415,16 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>3177</v>
+        <v>2875</v>
       </c>
       <c r="C14">
-        <v>6028</v>
+        <v>6040</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>24669</v>
+        <v>22008</v>
       </c>
       <c r="F14" t="s">
         <v>29</v>
@@ -3777,16 +3783,16 @@
         <v>1</v>
       </c>
       <c r="B27">
-        <v>3177</v>
+        <v>2875</v>
       </c>
       <c r="C27">
-        <v>6028</v>
+        <v>6040</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>24669</v>
+        <v>22008</v>
       </c>
       <c r="F27" t="s">
         <v>29</v>
@@ -4181,16 +4187,16 @@
         <v>1</v>
       </c>
       <c r="B40">
-        <v>3177</v>
+        <v>2875</v>
       </c>
       <c r="C40">
-        <v>6028</v>
+        <v>6040</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40">
-        <v>6028</v>
+        <v>6040</v>
       </c>
       <c r="F40" t="s">
         <v>29</v>

</xml_diff>